<commit_message>
prem past season data
</commit_message>
<xml_diff>
--- a/laliga2122tab.xlsx
+++ b/laliga2122tab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idrishedayat/Documents/STAT0035/DissertationOfficial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3A5B325-D4FA-D047-AC50-8F171621A013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A5FD3B7F-D74C-3E47-93CB-9207FB901A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15760"/>
   </bookViews>
@@ -974,7 +974,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="S1" activeCellId="8" sqref="K1:K1048576 L1:L1048576 O1:O1048576 M1:M1048576 N1:N1048576 Q1:Q1048576 P1:P1048576 R1:R1048576 S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>